<commit_message>
FO 1.0 | Logbook | Planning
FO 1.0 | Logbook | Planning
</commit_message>
<xml_diff>
--- a/Documentatie BeePlanner/Planning.xlsx
+++ b/Documentatie BeePlanner/Planning.xlsx
@@ -264,7 +264,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="dd/mm;@"/>
     <numFmt numFmtId="165" formatCode="dd\-mm\-yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="dd\.mm\.yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -652,6 +652,33 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="19" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="166" fontId="10" fillId="6" borderId="1" xfId="7" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="19" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="19" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -688,41 +715,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="6" borderId="1" xfId="7" applyNumberFormat="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="19" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="19" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1134,10 +1134,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO41"/>
+  <dimension ref="B1:BO40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1165,88 +1165,88 @@
       <c r="G1" s="11"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="37">
+      <c r="H2" s="25">
         <v>43234</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="35"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="44"/>
       <c r="Q2" s="18"/>
-      <c r="R2" s="33" t="s">
+      <c r="R2" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="34"/>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="35"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="43"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="44"/>
       <c r="Z2" s="14"/>
-      <c r="AA2" s="25" t="s">
+      <c r="AA2" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="36"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="45"/>
       <c r="AE2" s="15"/>
-      <c r="AF2" s="25" t="s">
+      <c r="AF2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AG2" s="26"/>
-      <c r="AH2" s="26"/>
-      <c r="AI2" s="26"/>
-      <c r="AJ2" s="26"/>
-      <c r="AK2" s="26"/>
-      <c r="AL2" s="26"/>
-      <c r="AM2" s="26"/>
-      <c r="AN2" s="36"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="35"/>
+      <c r="AJ2" s="35"/>
+      <c r="AK2" s="35"/>
+      <c r="AL2" s="35"/>
+      <c r="AM2" s="35"/>
+      <c r="AN2" s="45"/>
       <c r="AO2" s="16"/>
-      <c r="AP2" s="25" t="s">
+      <c r="AP2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="AQ2" s="26"/>
-      <c r="AR2" s="26"/>
-      <c r="AS2" s="26"/>
-      <c r="AT2" s="26"/>
-      <c r="AU2" s="26"/>
-      <c r="AV2" s="26"/>
-      <c r="AW2" s="26"/>
-      <c r="AX2" s="26"/>
+      <c r="AQ2" s="35"/>
+      <c r="AR2" s="35"/>
+      <c r="AS2" s="35"/>
+      <c r="AT2" s="35"/>
+      <c r="AU2" s="35"/>
+      <c r="AV2" s="35"/>
+      <c r="AW2" s="35"/>
+      <c r="AX2" s="35"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="30" t="s">
+      <c r="B3" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="41" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="17" t="s">
@@ -1273,12 +1273,12 @@
       <c r="AA3" s="9"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="29"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="19">
         <v>43234</v>
       </c>
@@ -1408,7 +1408,7 @@
       <c r="D5" s="22">
         <v>1</v>
       </c>
-      <c r="E5" s="48">
+      <c r="E5" s="33">
         <v>43234</v>
       </c>
       <c r="F5" s="6">
@@ -1429,7 +1429,7 @@
       <c r="D6" s="22">
         <v>30</v>
       </c>
-      <c r="E6" s="48">
+      <c r="E6" s="33">
         <v>43234</v>
       </c>
       <c r="F6" s="6"/>
@@ -1448,7 +1448,7 @@
       <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="48">
+      <c r="E7" s="33">
         <v>43234</v>
       </c>
       <c r="F7" s="6"/>
@@ -1466,7 +1466,7 @@
       <c r="D8" s="6">
         <v>2</v>
       </c>
-      <c r="E8" s="48"/>
+      <c r="E8" s="33"/>
       <c r="F8" s="6"/>
       <c r="G8" s="7">
         <v>0</v>
@@ -1489,7 +1489,7 @@
       </c>
     </row>
     <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="47" t="s">
+      <c r="B10" s="32" t="s">
         <v>37</v>
       </c>
       <c r="C10" s="20">
@@ -1505,7 +1505,7 @@
       </c>
     </row>
     <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="32" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="20">
@@ -1521,7 +1521,7 @@
       </c>
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="47" t="s">
+      <c r="B12" s="32" t="s">
         <v>38</v>
       </c>
       <c r="C12" s="20">
@@ -1537,7 +1537,7 @@
       </c>
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="32" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="20">
@@ -1553,7 +1553,7 @@
       </c>
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="32" t="s">
         <v>40</v>
       </c>
       <c r="C14" s="20">
@@ -1569,7 +1569,7 @@
       </c>
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="32" t="s">
         <v>42</v>
       </c>
       <c r="C15" s="20">
@@ -1585,7 +1585,7 @@
       </c>
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="32" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="20">
@@ -1601,7 +1601,7 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="32" t="s">
         <v>43</v>
       </c>
       <c r="C17" s="20">
@@ -1617,7 +1617,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="32" t="s">
         <v>51</v>
       </c>
       <c r="C18" s="20">
@@ -1633,7 +1633,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="47" t="s">
+      <c r="B19" s="32" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="20">
@@ -1649,7 +1649,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="32" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="20">
@@ -1665,7 +1665,7 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="32" t="s">
         <v>44</v>
       </c>
       <c r="C21" s="20">
@@ -1681,7 +1681,7 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="47" t="s">
+      <c r="B22" s="32" t="s">
         <v>35</v>
       </c>
       <c r="C22" s="20">
@@ -1697,7 +1697,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="32" t="s">
         <v>49</v>
       </c>
       <c r="C23" s="20">
@@ -1713,7 +1713,7 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="47" t="s">
+      <c r="B24" s="32" t="s">
         <v>36</v>
       </c>
       <c r="C24" s="20">
@@ -1729,7 +1729,7 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="47" t="s">
+      <c r="B25" s="32" t="s">
         <v>46</v>
       </c>
       <c r="C25" s="20">
@@ -1745,7 +1745,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="47" t="s">
+      <c r="B26" s="32" t="s">
         <v>45</v>
       </c>
       <c r="C26" s="20">
@@ -1761,7 +1761,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="47" t="s">
+      <c r="B27" s="32" t="s">
         <v>44</v>
       </c>
       <c r="C27" s="20">
@@ -1777,7 +1777,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="47" t="s">
+      <c r="B28" s="32" t="s">
         <v>48</v>
       </c>
       <c r="C28" s="20">
@@ -1793,7 +1793,7 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="47" t="s">
+      <c r="B29" s="32" t="s">
         <v>47</v>
       </c>
       <c r="C29" s="20">
@@ -1809,127 +1809,122 @@
       </c>
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="47"/>
+      <c r="B30" s="32"/>
       <c r="C30" s="20"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="47"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="7">
-        <v>0</v>
-      </c>
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="46">
+        <v>43234</v>
+      </c>
+      <c r="D31" s="46"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
     </row>
     <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="39">
-        <v>43234</v>
-      </c>
-      <c r="D32" s="39"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
+      <c r="B32" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
     </row>
     <row r="33" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
+      <c r="B33" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="27">
+        <v>211596</v>
+      </c>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
     </row>
     <row r="34" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="40">
-        <v>211596</v>
-      </c>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
+      <c r="B34" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
     </row>
     <row r="35" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="38"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
+      <c r="B35" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="26"/>
     </row>
     <row r="36" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="38"/>
+      <c r="B36" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
     </row>
     <row r="37" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="B37" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="28">
+        <v>95313</v>
+      </c>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
     </row>
     <row r="38" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="C38" s="42">
-        <v>95313</v>
-      </c>
-      <c r="D38" s="38"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
+      <c r="B38" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="48"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
     </row>
     <row r="39" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="44"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="45"/>
-    </row>
-    <row r="40" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="46" t="s">
+      <c r="B39" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="38" t="s">
+      <c r="C39" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-    </row>
-    <row r="41" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="24"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+    </row>
+    <row r="40" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="C38:D38"/>
     <mergeCell ref="AP2:AX2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
@@ -1942,13 +1937,8 @@
     <mergeCell ref="R2:Y2"/>
     <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="AF2:AN2"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C39:D39"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:BO31">
+  <conditionalFormatting sqref="H5:BO30">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1974,7 +1964,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G32:BO32">
+  <conditionalFormatting sqref="G31:BO31">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
FO & TO Changes, MVC Added
FO & TO Changes, MVC Added
</commit_message>
<xml_diff>
--- a/Documentatie BeePlanner/Planning.xlsx
+++ b/Documentatie BeePlanner/Planning.xlsx
@@ -215,9 +215,6 @@
     <t xml:space="preserve">Ontwikkelomgeving opzetten </t>
   </si>
   <si>
-    <t>User MVC en Route aanmaken</t>
-  </si>
-  <si>
     <t>Project MVC en Route aanmaken</t>
   </si>
   <si>
@@ -255,6 +252,9 @@
   </si>
   <si>
     <t>Vormgeving implementatie</t>
+  </si>
+  <si>
+    <t>Gebruiker MVC en Route aanmaken</t>
   </si>
 </sst>
 </file>
@@ -679,6 +679,42 @@
     <xf numFmtId="16" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -687,42 +723,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1136,8 +1136,8 @@
   </sheetPr>
   <dimension ref="B1:BO40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1165,13 +1165,13 @@
       <c r="G1" s="11"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
@@ -1179,74 +1179,74 @@
         <v>43234</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="45" t="s">
+      <c r="K2" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="47"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="44"/>
       <c r="Q2" s="18"/>
-      <c r="R2" s="45" t="s">
+      <c r="R2" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="46"/>
-      <c r="V2" s="46"/>
-      <c r="W2" s="46"/>
-      <c r="X2" s="46"/>
-      <c r="Y2" s="47"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="43"/>
+      <c r="V2" s="43"/>
+      <c r="W2" s="43"/>
+      <c r="X2" s="43"/>
+      <c r="Y2" s="44"/>
       <c r="Z2" s="14"/>
-      <c r="AA2" s="37" t="s">
+      <c r="AA2" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="38"/>
-      <c r="AC2" s="38"/>
-      <c r="AD2" s="48"/>
+      <c r="AB2" s="35"/>
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="45"/>
       <c r="AE2" s="15"/>
-      <c r="AF2" s="37" t="s">
+      <c r="AF2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="AG2" s="38"/>
-      <c r="AH2" s="38"/>
-      <c r="AI2" s="38"/>
-      <c r="AJ2" s="38"/>
-      <c r="AK2" s="38"/>
-      <c r="AL2" s="38"/>
-      <c r="AM2" s="38"/>
-      <c r="AN2" s="48"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="35"/>
+      <c r="AJ2" s="35"/>
+      <c r="AK2" s="35"/>
+      <c r="AL2" s="35"/>
+      <c r="AM2" s="35"/>
+      <c r="AN2" s="45"/>
       <c r="AO2" s="16"/>
-      <c r="AP2" s="37" t="s">
+      <c r="AP2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="AQ2" s="38"/>
-      <c r="AR2" s="38"/>
-      <c r="AS2" s="38"/>
-      <c r="AT2" s="38"/>
-      <c r="AU2" s="38"/>
-      <c r="AV2" s="38"/>
-      <c r="AW2" s="38"/>
-      <c r="AX2" s="38"/>
+      <c r="AQ2" s="35"/>
+      <c r="AR2" s="35"/>
+      <c r="AS2" s="35"/>
+      <c r="AT2" s="35"/>
+      <c r="AU2" s="35"/>
+      <c r="AV2" s="35"/>
+      <c r="AW2" s="35"/>
+      <c r="AX2" s="35"/>
     </row>
     <row r="3" spans="2:67" s="10" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="42" t="s">
+      <c r="B3" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="G3" s="41" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="17" t="s">
@@ -1273,12 +1273,12 @@
       <c r="AA3" s="9"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="41"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
       <c r="H4" s="19">
         <v>43234</v>
       </c>
@@ -1421,7 +1421,7 @@
     </row>
     <row r="6" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="20">
         <v>43234</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="32" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C12" s="20">
         <v>43241</v>
@@ -1540,7 +1540,7 @@
     </row>
     <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="20">
         <v>43244</v>
@@ -1556,7 +1556,7 @@
     </row>
     <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="20">
         <v>43247</v>
@@ -1572,7 +1572,7 @@
     </row>
     <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="20">
         <v>43248</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="20">
         <v>43249</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17" s="20">
         <v>43250</v>
@@ -1620,7 +1620,7 @@
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="20">
         <v>43251</v>
@@ -1636,7 +1636,7 @@
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="20">
         <v>43252</v>
@@ -1652,7 +1652,7 @@
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C20" s="20">
         <v>43253</v>
@@ -1668,7 +1668,7 @@
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="20">
         <v>43254</v>
@@ -1700,7 +1700,7 @@
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C23" s="20">
         <v>43256</v>
@@ -1732,7 +1732,7 @@
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="32" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C25" s="20">
         <v>43258</v>
@@ -1748,7 +1748,7 @@
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="20">
         <v>43259</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="20">
         <v>43260</v>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="20">
         <v>43261</v>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C29" s="20">
         <v>43262</v>
@@ -1822,10 +1822,10 @@
       <c r="B31" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="34">
+      <c r="C31" s="46">
         <v>43234</v>
       </c>
-      <c r="D31" s="34"/>
+      <c r="D31" s="46"/>
       <c r="E31" s="26"/>
       <c r="F31" s="26"/>
     </row>
@@ -1833,12 +1833,12 @@
       <c r="B32" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="35" t="s">
+      <c r="C32" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
     </row>
     <row r="33" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="27" t="s">
@@ -1866,23 +1866,23 @@
       <c r="B35" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="35" t="s">
+      <c r="C35" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
       <c r="F35" s="26"/>
     </row>
     <row r="36" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="35"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
     </row>
     <row r="37" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="28" t="s">
@@ -1899,10 +1899,10 @@
       <c r="B38" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="36" t="s">
+      <c r="C38" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="D38" s="36"/>
+      <c r="D38" s="48"/>
       <c r="E38" s="30"/>
       <c r="F38" s="30"/>
     </row>
@@ -1922,6 +1922,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="C38:D38"/>
     <mergeCell ref="AP2:AX2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
@@ -1934,11 +1939,6 @@
     <mergeCell ref="R2:Y2"/>
     <mergeCell ref="AA2:AD2"/>
     <mergeCell ref="AF2:AN2"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="C38:D38"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:BO30">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>